<commit_message>
pdf and new geodatabase upload
</commit_message>
<xml_diff>
--- a/Data/ME_Recipients.xlsx
+++ b/Data/ME_Recipients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor.z.lange/Library/CloudStorage/OneDrive-UniversityofMaineSystem/Research/Brownfields/Brownfields in Maine/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor.z.lange/Documents/GitHub/Maine_Brownfields/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352011D2-2CCD-D341-BD22-277CE40F9D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4700CA5-3CDA-2449-8D6F-126F51ED8D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="5020" windowWidth="30240" windowHeight="18880" xr2:uid="{4D949AB9-1976-46CE-8655-611C910AD3CD}"/>
+    <workbookView xWindow="-1480" yWindow="-20360" windowWidth="30240" windowHeight="18880" xr2:uid="{4D949AB9-1976-46CE-8655-611C910AD3CD}"/>
   </bookViews>
   <sheets>
     <sheet name="ME_Recipients" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="126">
   <si>
     <t>recipients</t>
   </si>
@@ -377,6 +377,27 @@
   </si>
   <si>
     <t xml:space="preserve">City of Biddeford                           </t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Federal</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Regional</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Tribal</t>
+  </si>
+  <si>
+    <t>County</t>
   </si>
 </sst>
 </file>
@@ -1237,823 +1258,1127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB78F597-70FD-4051-BACC-42A18C86208A}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>72</v>
       </c>
       <c r="B67" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>83</v>
       </c>
       <c r="B68" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>73</v>
       </c>
       <c r="B69" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>74</v>
       </c>
       <c r="B70" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>75</v>
       </c>
       <c r="B71" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>76</v>
       </c>
       <c r="B72" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>77</v>
       </c>
       <c r="B73" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>78</v>
       </c>
       <c r="B74" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>79</v>
       </c>
       <c r="B75" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>80</v>
       </c>
       <c r="B76" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>81</v>
       </c>
       <c r="B77" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>82</v>
       </c>
       <c r="B78" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>93</v>
       </c>
       <c r="B79" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>94</v>
       </c>
       <c r="B80" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>95</v>
       </c>
       <c r="B81" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>96</v>
       </c>
       <c r="B82" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>97</v>
       </c>
       <c r="B83" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>91</v>
       </c>
       <c r="B84" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>98</v>
       </c>
       <c r="B85" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>99</v>
       </c>
       <c r="B86" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>100</v>
       </c>
       <c r="B87" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>101</v>
       </c>
       <c r="B88" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>102</v>
       </c>
       <c r="B89" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>103</v>
       </c>
       <c r="B90" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>104</v>
       </c>
       <c r="B91" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>105</v>
       </c>
       <c r="B92" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>106</v>
       </c>
       <c r="B93" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>107</v>
       </c>
       <c r="B94" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>108</v>
       </c>
       <c r="B95" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>109</v>
       </c>
       <c r="B96" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>110</v>
       </c>
       <c r="B97" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>111</v>
       </c>
       <c r="B98" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>112</v>
       </c>
       <c r="B99" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>113</v>
       </c>
       <c r="B100" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C100" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>114</v>
       </c>
       <c r="B101" t="s">
         <v>86</v>
+      </c>
+      <c r="C101" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>